<commit_message>
variant based export (no gerber)
</commit_message>
<xml_diff>
--- a/HW/PCB_BOT/Default Configuration/Outputs/BOM/BOM_PartType-Timer_Clock_BOT(Alarm Clock).xlsx
+++ b/HW/PCB_BOT/Default Configuration/Outputs/BOM/BOM_PartType-Timer_Clock_BOT(Alarm Clock).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB410386-7FE7-4067-A35F-240B21982CD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BA638369-6E29-4530-B75C-29CA82ACFD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{9869CE9A-9B50-4F82-BBE4-C3A0B6E784BA}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{C2EBFBBF-34C0-4A4E-AD10-83F261DCCE48}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-Timer_Clock_BOT(Al" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="257">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="267">
   <si>
     <t>Quantity</t>
   </si>
@@ -141,58 +141,73 @@
     <t>CAP_100nF_10V_0402</t>
   </si>
   <si>
-    <t>J200</t>
+    <t>J202</t>
   </si>
   <si>
     <t>Connector</t>
   </si>
   <si>
-    <t>2x1</t>
-  </si>
-  <si>
-    <t>CONN HEADER VERT 2POS 2.54MM</t>
+    <t>TYPE-C-31-M-17</t>
+  </si>
+  <si>
+    <t>USB4 GEN3, TYPE C, TOP MOUNT</t>
+  </si>
+  <si>
+    <t>Korean Hroparts Elec</t>
+  </si>
+  <si>
+    <t>J_USB-C_2</t>
+  </si>
+  <si>
+    <t>J300</t>
+  </si>
+  <si>
+    <t>PH2</t>
+  </si>
+  <si>
+    <t>CONN HEADER R/A 2POS 2MM</t>
+  </si>
+  <si>
+    <t>JST Sales America Inc.</t>
+  </si>
+  <si>
+    <t>S2B-PH-KL(LF)(SN)</t>
+  </si>
+  <si>
+    <t>J_S2B-PH-KL</t>
+  </si>
+  <si>
+    <t>J301</t>
+  </si>
+  <si>
+    <t>CON</t>
+  </si>
+  <si>
+    <t>CONN CONNECTOR PH 2POS 2MM</t>
+  </si>
+  <si>
+    <t>PHR-2-R</t>
+  </si>
+  <si>
+    <t>J_PHR-2-R</t>
+  </si>
+  <si>
+    <t>J305</t>
+  </si>
+  <si>
+    <t>5x2</t>
+  </si>
+  <si>
+    <t>CONN HEADER SMD 10POS 1.27MM</t>
   </si>
   <si>
     <t>Sullins Connector Solutions</t>
   </si>
   <si>
-    <t>PRPC002SAAN-RC</t>
-  </si>
-  <si>
-    <t>J_MH2x1_2.54</t>
-  </si>
-  <si>
-    <t>J202</t>
-  </si>
-  <si>
-    <t>TYPE-C-31-M-17</t>
-  </si>
-  <si>
-    <t>USB4 GEN3, TYPE C, TOP MOUNT</t>
-  </si>
-  <si>
-    <t>Korean Hroparts Elec</t>
-  </si>
-  <si>
-    <t>J_USB-C_2</t>
-  </si>
-  <si>
-    <t>J301</t>
-  </si>
-  <si>
-    <t>CON</t>
-  </si>
-  <si>
-    <t>CONN CONNECTOR PH 2POS 2MM</t>
-  </si>
-  <si>
-    <t>JST Sales America Inc.</t>
-  </si>
-  <si>
-    <t>PHR-2-R</t>
-  </si>
-  <si>
-    <t>J_PHR-2-R</t>
+    <t>GRPB052VWQS-RC</t>
+  </si>
+  <si>
+    <t>J_MH5x2_1.27</t>
   </si>
   <si>
     <t>J400</t>
@@ -213,21 +228,6 @@
     <t>J_FPC24_DS</t>
   </si>
   <si>
-    <t>J205, J300</t>
-  </si>
-  <si>
-    <t>PH2</t>
-  </si>
-  <si>
-    <t>CONN HEADER R/A 2POS 2MM</t>
-  </si>
-  <si>
-    <t>S2B-PH-KL(LF)(SN)</t>
-  </si>
-  <si>
-    <t>J_S2B-PH-KL</t>
-  </si>
-  <si>
     <t>J302, J303</t>
   </si>
   <si>
@@ -396,7 +396,7 @@
     <t>IC, EEPROM</t>
   </si>
   <si>
-    <t>EEPROM 4Kb</t>
+    <t>AT34C04-X5M</t>
   </si>
   <si>
     <t>IC EEPROM 4KBIT I2C 1MHZ 8TSSOP</t>
@@ -408,7 +408,7 @@
     <t>AT34C04-X5M-T</t>
   </si>
   <si>
-    <t>IC_EEPROM_4Kb</t>
+    <t>IC_EEPROM_AT34C04</t>
   </si>
   <si>
     <t>IC302</t>
@@ -573,6 +573,24 @@
     <t>J_BAT_CLIP_18650_B</t>
   </si>
   <si>
+    <t>SW302</t>
+  </si>
+  <si>
+    <t>SW</t>
+  </si>
+  <si>
+    <t>SWITCH TACTILE SPST-NO 0.05A 16V</t>
+  </si>
+  <si>
+    <t>C&amp;K</t>
+  </si>
+  <si>
+    <t>PTS810 SJM 250 SMTR LFS</t>
+  </si>
+  <si>
+    <t>SW_TactileSW_V</t>
+  </si>
+  <si>
     <t>Q300</t>
   </si>
   <si>
@@ -654,25 +672,25 @@
     <t>R_84k5_0402</t>
   </si>
   <si>
-    <t>SW302</t>
-  </si>
-  <si>
-    <t>SW</t>
-  </si>
-  <si>
-    <t>SWITCH TACTILE SPST-NO 0.05A 16V</t>
-  </si>
-  <si>
-    <t>C&amp;K</t>
-  </si>
-  <si>
-    <t>PTS810 SJM 250 SMTR LFS</t>
-  </si>
-  <si>
-    <t>SW_TactileSW_V</t>
-  </si>
-  <si>
-    <t>R203, R205, R208, R209, R210, R214, R215, R300, R301, R302, R303, R304, R305, R306, R307, R312</t>
+    <t>R401</t>
+  </si>
+  <si>
+    <t>R 1k8 0402</t>
+  </si>
+  <si>
+    <t>RES 100K OHM 5% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>YAGEO</t>
+  </si>
+  <si>
+    <t>RC0402JR-07100KL</t>
+  </si>
+  <si>
+    <t>R_100k_0402</t>
+  </si>
+  <si>
+    <t>R203, R205, R208, R209, R210, R214, R215, R300, R301, R302, R303, R304, R305, R306, R307, R312, R319, R320</t>
   </si>
   <si>
     <t>R 10k 0402</t>
@@ -681,9 +699,6 @@
     <t>RES 10K OHM 1% 1/16W 0402</t>
   </si>
   <si>
-    <t>YAGEO</t>
-  </si>
-  <si>
     <t>RC0402FR-0710KL</t>
   </si>
   <si>
@@ -705,6 +720,21 @@
     <t>R_5k1_0420</t>
   </si>
   <si>
+    <t>R218, R219, R402</t>
+  </si>
+  <si>
+    <t>R 0R0 0402</t>
+  </si>
+  <si>
+    <t>RES 0 OHM JUMPER 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RMCF0402ZT0R00</t>
+  </si>
+  <si>
+    <t>R_0R0_0402</t>
+  </si>
+  <si>
     <t>R200, R201, R216, R310</t>
   </si>
   <si>
@@ -720,7 +750,22 @@
     <t>R_270k_0402</t>
   </si>
   <si>
-    <t>R202, R315, R316, R317, R318</t>
+    <t>R204, R206, R207, R308, R309, R311, R313, R314</t>
+  </si>
+  <si>
+    <t>R 2k 0402</t>
+  </si>
+  <si>
+    <t>RES 2K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RMCF0402FT2K00</t>
+  </si>
+  <si>
+    <t>R_2k_0402</t>
+  </si>
+  <si>
+    <t>R202, R315, R316, R317, R318, R321, R322, R323, R324</t>
   </si>
   <si>
     <t>R 100R 0402</t>
@@ -735,21 +780,6 @@
     <t>R_100R_0402</t>
   </si>
   <si>
-    <t>R204, R206, R207, R308, R309, R311, R313, R314</t>
-  </si>
-  <si>
-    <t>R 2k 0402</t>
-  </si>
-  <si>
-    <t>RES 2K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>RMCF0402FT2K00</t>
-  </si>
-  <si>
-    <t>R_2k_0402</t>
-  </si>
-  <si>
     <t>P200</t>
   </si>
   <si>
@@ -771,7 +801,7 @@
     <t>P_2NCH_20V_1W</t>
   </si>
   <si>
-    <t>P300</t>
+    <t>P300, P400</t>
   </si>
   <si>
     <t>P PMOS 30V 6A</t>
@@ -1181,8 +1211,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC0755D8-C512-4423-B0D8-B376ED26C77E}">
-  <dimension ref="A1:H43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7082B519-131C-44FD-AEC8-25A3D0865D03}">
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1373,10 +1403,10 @@
         <v>41</v>
       </c>
       <c r="G7" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -1384,22 +1414,22 @@
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="F8" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="G8" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>48</v>
@@ -1422,13 +1452,13 @@
         <v>51</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G9" s="3" t="s">
+      <c r="H9" s="3" t="s">
         <v>53</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -1436,45 +1466,45 @@
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>59</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>38</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E11" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E11" s="3" t="s">
+      <c r="F11" s="3" t="s">
         <v>63</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="G11" s="3" t="s">
         <v>64</v>
@@ -1500,7 +1530,7 @@
         <v>68</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>69</v>
@@ -1985,74 +2015,74 @@
         <v>181</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="E31" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="E31" s="3" t="s">
+      <c r="F31" s="3" t="s">
         <v>184</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="G31" s="3" t="s">
+      <c r="H31" s="3" t="s">
         <v>186</v>
-      </c>
-      <c r="H31" s="3" t="s">
-        <v>187</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B32" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="D32" s="3" t="s">
         <v>189</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="E32" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="E32" s="3" t="s">
+      <c r="F32" s="3" t="s">
         <v>191</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="G32" s="3" t="s">
         <v>192</v>
       </c>
-      <c r="G32" s="3" t="s">
+      <c r="H32" s="3" t="s">
         <v>193</v>
-      </c>
-      <c r="H32" s="3" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B33" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>195</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="D33" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D33" s="3" t="s">
+      <c r="E33" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="E33" s="3" t="s">
+      <c r="F33" s="3" t="s">
         <v>198</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="G33" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="G33" s="3" t="s">
+      <c r="H33" s="3" t="s">
         <v>200</v>
-      </c>
-      <c r="H33" s="3" t="s">
-        <v>201</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -2060,10 +2090,10 @@
         <v>1</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>202</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>203</v>
@@ -2089,7 +2119,7 @@
         <v>208</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>209</v>
@@ -2109,13 +2139,13 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>214</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>215</v>
@@ -2135,13 +2165,13 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>2</v>
+        <v>18</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>220</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>221</v>
@@ -2150,7 +2180,7 @@
         <v>222</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="G37" s="3" t="s">
         <v>223</v>
@@ -2161,13 +2191,13 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>225</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D38" s="3" t="s">
         <v>226</v>
@@ -2176,7 +2206,7 @@
         <v>227</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>228</v>
@@ -2187,13 +2217,13 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>230</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>231</v>
@@ -2202,7 +2232,7 @@
         <v>232</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="G39" s="3" t="s">
         <v>233</v>
@@ -2213,13 +2243,13 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>235</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="D40" s="3" t="s">
         <v>236</v>
@@ -2228,7 +2258,7 @@
         <v>237</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>199</v>
+        <v>217</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>238</v>
@@ -2239,80 +2269,132 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>240</v>
       </c>
       <c r="C41" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>241</v>
       </c>
-      <c r="D41" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="E41" s="3" t="s">
+      <c r="F41" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="G41" s="3" t="s">
         <v>243</v>
       </c>
-      <c r="F41" s="3" t="s">
+      <c r="H41" s="3" t="s">
         <v>244</v>
-      </c>
-      <c r="G41" s="3" t="s">
-        <v>245</v>
-      </c>
-      <c r="H41" s="3" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B42" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="E42" s="3" t="s">
         <v>247</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="D42" s="3" t="s">
+      <c r="F42" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="G42" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="E42" s="3" t="s">
+      <c r="H42" s="3" t="s">
         <v>249</v>
-      </c>
-      <c r="F42" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="G42" s="3" t="s">
-        <v>250</v>
-      </c>
-      <c r="H42" s="3" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
+        <v>1</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="F43" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="G43" s="3" t="s">
+        <v>255</v>
+      </c>
+      <c r="H43" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>2</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="F44" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
         <v>3</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>252</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="D43" s="3" t="s">
-        <v>253</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>254</v>
-      </c>
-      <c r="F43" s="3" t="s">
-        <v>255</v>
-      </c>
-      <c r="G43" s="3" t="s">
-        <v>256</v>
-      </c>
-      <c r="H43" s="3" t="s">
-        <v>253</v>
+      <c r="B45" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="F45" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="G45" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="H45" s="3" t="s">
+        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ready for manufacturing (V2.0)
</commit_message>
<xml_diff>
--- a/HW/PCB_BOT/Default Configuration/Outputs/BOM/BOM_PartType-Timer_Clock_BOT(Alarm Clock).xlsx
+++ b/HW/PCB_BOT/Default Configuration/Outputs/BOM/BOM_PartType-Timer_Clock_BOT(Alarm Clock).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0189538D-1333-43A7-BCD7-AF0851F906C7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{165F60BA-B36E-416E-8C2F-A4FCDAA6EA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{5D0AFE67-5903-48AC-85F0-0B4E2B7F3398}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{DA7641F8-5490-4664-828E-5E0567AF8CE3}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-Timer_Clock_BOT(Al" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="316">
   <si>
     <t>Quantity</t>
   </si>
@@ -54,6 +54,12 @@
     <t>LibRef</t>
   </si>
   <si>
+    <t>Supplier 1</t>
+  </si>
+  <si>
+    <t>Supplier Part Number 1</t>
+  </si>
+  <si>
     <t>C200</t>
   </si>
   <si>
@@ -75,6 +81,12 @@
     <t>CAP_1nF_50V_0402</t>
   </si>
   <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>490-6190-1-ND</t>
+  </si>
+  <si>
     <t>C307, C308</t>
   </si>
   <si>
@@ -93,6 +105,9 @@
     <t>CAP_5.6PF_50V_0402</t>
   </si>
   <si>
+    <t>1276-1712-1-ND</t>
+  </si>
+  <si>
     <t>C201, C202, C203, C208</t>
   </si>
   <si>
@@ -111,6 +126,9 @@
     <t>CAP_10uF_6V3_0603</t>
   </si>
   <si>
+    <t>587-5869-1-ND</t>
+  </si>
+  <si>
     <t>C300, C301, C302, C303, C304</t>
   </si>
   <si>
@@ -126,6 +144,9 @@
     <t>CAP_10nF_16V_0402</t>
   </si>
   <si>
+    <t>1276-1738-1-ND</t>
+  </si>
+  <si>
     <t>C204, C205, C206, C207, C209, C305, C306, C400</t>
   </si>
   <si>
@@ -141,6 +162,9 @@
     <t>CAP_100nF_10V_0402</t>
   </si>
   <si>
+    <t>1276-1443-1-ND</t>
+  </si>
+  <si>
     <t>J202</t>
   </si>
   <si>
@@ -159,6 +183,12 @@
     <t>J_USB-C_2</t>
   </si>
   <si>
+    <t>LCSC</t>
+  </si>
+  <si>
+    <t>C283540</t>
+  </si>
+  <si>
     <t>J300</t>
   </si>
   <si>
@@ -177,6 +207,9 @@
     <t>J_S2B-PH-KL</t>
   </si>
   <si>
+    <t>C160237</t>
+  </si>
+  <si>
     <t>J301</t>
   </si>
   <si>
@@ -192,6 +225,9 @@
     <t>J_PHR-2-R</t>
   </si>
   <si>
+    <t>C398543</t>
+  </si>
+  <si>
     <t>J305</t>
   </si>
   <si>
@@ -210,6 +246,9 @@
     <t>J_MH5x2_1.27</t>
   </si>
   <si>
+    <t>S9012E-05-ND</t>
+  </si>
+  <si>
     <t>J400</t>
   </si>
   <si>
@@ -228,6 +267,9 @@
     <t>J_FPC24_DS</t>
   </si>
   <si>
+    <t>C293627</t>
+  </si>
+  <si>
     <t>J302, J303</t>
   </si>
   <si>
@@ -243,6 +285,9 @@
     <t>J_PHR-2-R_PIN</t>
   </si>
   <si>
+    <t>C160351</t>
+  </si>
+  <si>
     <t>D300, D301</t>
   </si>
   <si>
@@ -261,6 +306,9 @@
     <t>D_LL_200V_200mA</t>
   </si>
   <si>
+    <t>BAS20LT3GOSCT-ND</t>
+  </si>
+  <si>
     <t>D400, D401</t>
   </si>
   <si>
@@ -279,6 +327,9 @@
     <t>D_SCH_40V_5A</t>
   </si>
   <si>
+    <t>641-1126-1-ND</t>
+  </si>
+  <si>
     <t>D201</t>
   </si>
   <si>
@@ -300,6 +351,9 @@
     <t>D_LED_Green_0603</t>
   </si>
   <si>
+    <t>475-3442-1-ND</t>
+  </si>
+  <si>
     <t>D202, D302</t>
   </si>
   <si>
@@ -318,6 +372,9 @@
     <t>D_LED_Yellow_0603</t>
   </si>
   <si>
+    <t>404-1273-1-ND</t>
+  </si>
+  <si>
     <t>D200</t>
   </si>
   <si>
@@ -336,6 +393,9 @@
     <t>D_TVS_U4_12V5</t>
   </si>
   <si>
+    <t>641-1829-1-ND</t>
+  </si>
+  <si>
     <t>IC200</t>
   </si>
   <si>
@@ -354,6 +414,9 @@
     <t>IC_BAT_PROT_DW01A</t>
   </si>
   <si>
+    <t>C351410</t>
+  </si>
+  <si>
     <t>IC201</t>
   </si>
   <si>
@@ -372,6 +435,9 @@
     <t>IC_BAT_CHGR_TP4056</t>
   </si>
   <si>
+    <t>C16581</t>
+  </si>
+  <si>
     <t>IC400</t>
   </si>
   <si>
@@ -390,6 +456,9 @@
     <t>IC_16ch_Port_Extender_2</t>
   </si>
   <si>
+    <t>SX1503I091CT-ND</t>
+  </si>
+  <si>
     <t>IC301</t>
   </si>
   <si>
@@ -411,6 +480,9 @@
     <t>IC_EEPROM_AT34C04</t>
   </si>
   <si>
+    <t>AT34C04-X5M-TCT-ND</t>
+  </si>
+  <si>
     <t>IC302</t>
   </si>
   <si>
@@ -429,6 +501,9 @@
     <t>IC_MCU_STM32G031F8P6</t>
   </si>
   <si>
+    <t>C529334</t>
+  </si>
+  <si>
     <t>IC202</t>
   </si>
   <si>
@@ -444,6 +519,9 @@
     <t>IC_OpAmp_MCP6007-E/SN</t>
   </si>
   <si>
+    <t>150-MCP6007-E/SN-ND</t>
+  </si>
+  <si>
     <t>IC204</t>
   </si>
   <si>
@@ -465,6 +543,9 @@
     <t>IC_Ref_LM4040DIM3X-3.0</t>
   </si>
   <si>
+    <t>296-41429-1-ND</t>
+  </si>
+  <si>
     <t>IC203</t>
   </si>
   <si>
@@ -486,6 +567,9 @@
     <t>IC_Reg_TCR2LF30</t>
   </si>
   <si>
+    <t>TCR2LF30LM(CTCT-ND</t>
+  </si>
+  <si>
     <t>IC300</t>
   </si>
   <si>
@@ -507,6 +591,12 @@
     <t>IC_RTC_3028-C7</t>
   </si>
   <si>
+    <t>Mouser</t>
+  </si>
+  <si>
+    <t>428-203591-MG01</t>
+  </si>
+  <si>
     <t>L200</t>
   </si>
   <si>
@@ -528,6 +618,9 @@
     <t>L_100R_4A</t>
   </si>
   <si>
+    <t>283-MFBM1V3216-101-RCT-ND</t>
+  </si>
+  <si>
     <t>DS300</t>
   </si>
   <si>
@@ -549,6 +642,12 @@
     <t>DFP_Player_mini</t>
   </si>
   <si>
+    <t>AliExpress</t>
+  </si>
+  <si>
+    <t>33036928283</t>
+  </si>
+  <si>
     <t>J203</t>
   </si>
   <si>
@@ -567,6 +666,9 @@
     <t>J_BAT_CLIP_18650_A</t>
   </si>
   <si>
+    <t>C2979182</t>
+  </si>
+  <si>
     <t>J204</t>
   </si>
   <si>
@@ -591,6 +693,9 @@
     <t>SW_TactileSW_V</t>
   </si>
   <si>
+    <t>CKN10502CT-ND</t>
+  </si>
+  <si>
     <t>Q300</t>
   </si>
   <si>
@@ -612,6 +717,9 @@
     <t>Q_32k768_12p5</t>
   </si>
   <si>
+    <t>644-1313-1-ND</t>
+  </si>
+  <si>
     <t>SW300, SW301</t>
   </si>
   <si>
@@ -633,6 +741,9 @@
     <t>ENC_12_THT</t>
   </si>
   <si>
+    <t>PEC11R-4220F-S0012-ND</t>
+  </si>
+  <si>
     <t>R213</t>
   </si>
   <si>
@@ -654,6 +765,9 @@
     <t>R_220R_0603</t>
   </si>
   <si>
+    <t>RMCF0603FT220RCT-ND</t>
+  </si>
+  <si>
     <t>R217</t>
   </si>
   <si>
@@ -672,6 +786,9 @@
     <t>R_84k5_0402</t>
   </si>
   <si>
+    <t>541-84.5KLCT-ND</t>
+  </si>
+  <si>
     <t>R401</t>
   </si>
   <si>
@@ -690,6 +807,9 @@
     <t>R_100k_0402</t>
   </si>
   <si>
+    <t>311-100KJRCT-ND</t>
+  </si>
+  <si>
     <t>R203, R205, R208, R209, R210, R214, R215, R300, R301, R302, R303, R304, R305, R306, R307, R312, R319, R320</t>
   </si>
   <si>
@@ -705,6 +825,9 @@
     <t>R_10k_0402</t>
   </si>
   <si>
+    <t>311-10.0KLRCT-ND</t>
+  </si>
+  <si>
     <t>R211, R212</t>
   </si>
   <si>
@@ -720,6 +843,9 @@
     <t>R_5k1_0420</t>
   </si>
   <si>
+    <t>RMCF0402FT5K10CT-ND</t>
+  </si>
+  <si>
     <t>R218, R219, R402</t>
   </si>
   <si>
@@ -735,6 +861,9 @@
     <t>R_0R0_0402</t>
   </si>
   <si>
+    <t>RMCF0402ZT0R00CT-ND</t>
+  </si>
+  <si>
     <t>R200, R201, R216, R310</t>
   </si>
   <si>
@@ -750,6 +879,9 @@
     <t>R_270k_0402</t>
   </si>
   <si>
+    <t>311-270KLRCT-ND</t>
+  </si>
+  <si>
     <t>R204, R206, R207, R308, R309, R311, R313, R314</t>
   </si>
   <si>
@@ -765,6 +897,9 @@
     <t>R_2k_0402</t>
   </si>
   <si>
+    <t>RMCF0402FT2K00CT-ND</t>
+  </si>
+  <si>
     <t>R202, R315, R316, R317, R318, R321, R322, R323, R324</t>
   </si>
   <si>
@@ -780,6 +915,9 @@
     <t>R_100R_0402</t>
   </si>
   <si>
+    <t>RMCF0402FT100RCT-ND</t>
+  </si>
+  <si>
     <t>P200</t>
   </si>
   <si>
@@ -801,6 +939,9 @@
     <t>P_2NCH_20V_1W</t>
   </si>
   <si>
+    <t>C16052</t>
+  </si>
+  <si>
     <t>P300, P400</t>
   </si>
   <si>
@@ -816,6 +957,9 @@
     <t>P_PCH_30V_1W</t>
   </si>
   <si>
+    <t>SSM3J372RLFCT-ND</t>
+  </si>
+  <si>
     <t>P201, P202, P301</t>
   </si>
   <si>
@@ -829,6 +973,9 @@
   </si>
   <si>
     <t>RU1J002YNTCL</t>
+  </si>
+  <si>
+    <t>RU1J002YNTCLCT-ND</t>
   </si>
 </sst>
 </file>
@@ -1211,8 +1358,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3CB9195-B803-4C23-9380-94F62B26A416}">
-  <dimension ref="A1:H45"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C4F5D5-517E-4EF1-A569-6450CD80B884}">
+  <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1225,9 +1372,10 @@
     <col min="5" max="5" width="28.5703125" customWidth="1"/>
     <col min="6" max="7" width="13.28515625" customWidth="1"/>
     <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="10" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1252,1149 +1400,1419 @@
       <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>8</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>50</v>
+        <v>61</v>
       </c>
       <c r="E9" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J9" s="3" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>1</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>54</v>
+        <v>66</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>57</v>
+        <v>69</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>58</v>
+        <v>70</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>71</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>1</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>63</v>
+        <v>76</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>64</v>
+        <v>77</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>2</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>66</v>
+        <v>80</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>67</v>
+        <v>81</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>68</v>
+        <v>82</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>46</v>
+        <v>56</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>2</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+      <c r="I13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>2</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>78</v>
+        <v>94</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>79</v>
+        <v>95</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>80</v>
+        <v>96</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>81</v>
+        <v>97</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>1</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>83</v>
+        <v>100</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>85</v>
+        <v>102</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>86</v>
+        <v>103</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>87</v>
+        <v>104</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>2</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>84</v>
+        <v>101</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>91</v>
+        <v>109</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>92</v>
+        <v>110</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>93</v>
+        <v>111</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>94</v>
+        <v>112</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>1</v>
       </c>
       <c r="B17" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="F17" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D17" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="E17" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="F17" s="3" t="s">
-        <v>80</v>
-      </c>
       <c r="G17" s="3" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>1</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>102</v>
+        <v>122</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>105</v>
+        <v>125</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>106</v>
+        <v>126</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>104</v>
+        <v>124</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>127</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>1</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>108</v>
+        <v>129</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>109</v>
+        <v>130</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>110</v>
+        <v>131</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>111</v>
+        <v>132</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>134</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>1</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>114</v>
+        <v>136</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>115</v>
+        <v>137</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>118</v>
+        <v>140</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>116</v>
+        <v>138</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>141</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>1</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>120</v>
+        <v>143</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>121</v>
+        <v>144</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>122</v>
+        <v>145</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>123</v>
+        <v>146</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>125</v>
+        <v>148</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>149</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>1</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>128</v>
+        <v>152</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>131</v>
+        <v>155</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>129</v>
+        <v>153</v>
       </c>
       <c r="H22" s="3" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>156</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>1</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>133</v>
+        <v>158</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>134</v>
+        <v>159</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>136</v>
+        <v>161</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>124</v>
+        <v>147</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="H23" s="3" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+        <v>162</v>
+      </c>
+      <c r="I23" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>1</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>138</v>
+        <v>164</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>140</v>
+        <v>166</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>141</v>
+        <v>167</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>142</v>
+        <v>168</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>143</v>
+        <v>169</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+        <v>170</v>
+      </c>
+      <c r="I24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>1</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>145</v>
+        <v>172</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>146</v>
+        <v>173</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>147</v>
+        <v>174</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>148</v>
+        <v>175</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>150</v>
+        <v>177</v>
       </c>
       <c r="H25" s="3" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>178</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>1</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>152</v>
+        <v>180</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>153</v>
+        <v>181</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>154</v>
+        <v>182</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>155</v>
+        <v>183</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>156</v>
+        <v>184</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>157</v>
+        <v>185</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+        <v>186</v>
+      </c>
+      <c r="I26" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>1</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>159</v>
+        <v>189</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>160</v>
+        <v>190</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>161</v>
+        <v>191</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>162</v>
+        <v>192</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>163</v>
+        <v>193</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>164</v>
+        <v>194</v>
       </c>
       <c r="H27" s="3" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>195</v>
+      </c>
+      <c r="I27" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>1</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>166</v>
+        <v>197</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>167</v>
+        <v>198</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>168</v>
+        <v>199</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>169</v>
+        <v>200</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>172</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>203</v>
+      </c>
+      <c r="I28" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>1</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>173</v>
+        <v>206</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>167</v>
+        <v>198</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>174</v>
+        <v>207</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>175</v>
+        <v>208</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>176</v>
+        <v>209</v>
       </c>
       <c r="G29" s="3" t="s">
-        <v>177</v>
+        <v>210</v>
       </c>
       <c r="H29" s="3" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>211</v>
+      </c>
+      <c r="I29" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>1</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>179</v>
+        <v>213</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>167</v>
+        <v>198</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>174</v>
+        <v>207</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>175</v>
+        <v>208</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>176</v>
+        <v>209</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>177</v>
+        <v>210</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>214</v>
+      </c>
+      <c r="I30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>1</v>
       </c>
       <c r="B31" s="3" t="s">
-        <v>181</v>
+        <v>215</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>167</v>
+        <v>198</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>182</v>
+        <v>216</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>183</v>
+        <v>217</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>184</v>
+        <v>218</v>
       </c>
       <c r="G31" s="3" t="s">
-        <v>185</v>
+        <v>219</v>
       </c>
       <c r="H31" s="3" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>220</v>
+      </c>
+      <c r="I31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>1</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>187</v>
+        <v>222</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>188</v>
+        <v>223</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>189</v>
+        <v>224</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>190</v>
+        <v>225</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>191</v>
+        <v>226</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>192</v>
+        <v>227</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>228</v>
+      </c>
+      <c r="I32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>2</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>194</v>
+        <v>230</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>195</v>
+        <v>231</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>196</v>
+        <v>232</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>197</v>
+        <v>233</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>198</v>
+        <v>234</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>199</v>
+        <v>235</v>
       </c>
       <c r="H33" s="3" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>236</v>
+      </c>
+      <c r="I33" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>1</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>201</v>
+        <v>238</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>202</v>
+        <v>239</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>203</v>
+        <v>240</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>204</v>
+        <v>241</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>205</v>
+        <v>242</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>206</v>
+        <v>243</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>244</v>
+      </c>
+      <c r="I34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J34" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>1</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>208</v>
+        <v>246</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>202</v>
+        <v>239</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>209</v>
+        <v>247</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>210</v>
+        <v>248</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>211</v>
+        <v>249</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>212</v>
+        <v>250</v>
       </c>
       <c r="H35" s="3" t="s">
-        <v>213</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>251</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>1</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>214</v>
+        <v>253</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>202</v>
+        <v>239</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>215</v>
+        <v>254</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>216</v>
+        <v>255</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>217</v>
+        <v>256</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>218</v>
+        <v>257</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>258</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>18</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>220</v>
+        <v>260</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>202</v>
+        <v>239</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>221</v>
+        <v>261</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>222</v>
+        <v>262</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>217</v>
+        <v>256</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>223</v>
+        <v>263</v>
       </c>
       <c r="H37" s="3" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>264</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>2</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>225</v>
+        <v>266</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>202</v>
+        <v>239</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>226</v>
+        <v>267</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>227</v>
+        <v>268</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>205</v>
+        <v>242</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>228</v>
+        <v>269</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>229</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>270</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>3</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>230</v>
+        <v>272</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>202</v>
+        <v>239</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>231</v>
+        <v>273</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>232</v>
+        <v>274</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>205</v>
+        <v>242</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>233</v>
+        <v>275</v>
       </c>
       <c r="H39" s="3" t="s">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>276</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>4</v>
       </c>
       <c r="B40" s="3" t="s">
-        <v>235</v>
+        <v>278</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>202</v>
+        <v>239</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>236</v>
+        <v>279</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>237</v>
+        <v>280</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>217</v>
+        <v>256</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>238</v>
+        <v>281</v>
       </c>
       <c r="H40" s="3" t="s">
-        <v>239</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>282</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>8</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>240</v>
+        <v>284</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>202</v>
+        <v>239</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>241</v>
+        <v>285</v>
       </c>
       <c r="E41" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="F41" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>205</v>
-      </c>
       <c r="G41" s="3" t="s">
-        <v>243</v>
+        <v>287</v>
       </c>
       <c r="H41" s="3" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>288</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>9</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>245</v>
+        <v>290</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>202</v>
+        <v>239</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>246</v>
+        <v>291</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>247</v>
+        <v>292</v>
       </c>
       <c r="F42" s="3" t="s">
-        <v>205</v>
+        <v>242</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>248</v>
+        <v>293</v>
       </c>
       <c r="H42" s="3" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>294</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>1</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>250</v>
+        <v>296</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>251</v>
+        <v>297</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>252</v>
+        <v>298</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>253</v>
+        <v>299</v>
       </c>
       <c r="F43" s="3" t="s">
-        <v>254</v>
+        <v>300</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>255</v>
+        <v>301</v>
       </c>
       <c r="H43" s="3" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>302</v>
+      </c>
+      <c r="I43" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>2</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>257</v>
+        <v>304</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>251</v>
+        <v>297</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>258</v>
+        <v>305</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>259</v>
+        <v>306</v>
       </c>
       <c r="F44" s="3" t="s">
-        <v>149</v>
+        <v>176</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>260</v>
+        <v>307</v>
       </c>
       <c r="H44" s="3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>308</v>
+      </c>
+      <c r="I44" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>3</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>262</v>
+        <v>310</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>251</v>
+        <v>297</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>263</v>
+        <v>311</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>264</v>
+        <v>312</v>
       </c>
       <c r="F45" s="3" t="s">
-        <v>265</v>
+        <v>313</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>266</v>
+        <v>314</v>
       </c>
       <c r="H45" s="3" t="s">
-        <v>263</v>
+        <v>311</v>
+      </c>
+      <c r="I45" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>315</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
regenerated outputs after BOM change
</commit_message>
<xml_diff>
--- a/HW/PCB_BOT/Default Configuration/Outputs/BOM/BOM_PartType-Timer_Clock_BOT(Alarm Clock).xlsx
+++ b/HW/PCB_BOT/Default Configuration/Outputs/BOM/BOM_PartType-Timer_Clock_BOT(Alarm Clock).xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{165F60BA-B36E-416E-8C2F-A4FCDAA6EA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C6A0E3AA-BDA1-4B10-9487-68296FBA1EDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="28800" windowHeight="15435" xr2:uid="{DA7641F8-5490-4664-828E-5E0567AF8CE3}"/>
+    <workbookView xWindow="5115" yWindow="5565" windowWidth="28800" windowHeight="15435" xr2:uid="{31F48390-C06E-47DA-8EF8-A29908526343}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM_PartType-Timer_Clock_BOT(Al" sheetId="1" r:id="rId1"/>
@@ -60,12 +60,54 @@
     <t>Supplier Part Number 1</t>
   </si>
   <si>
-    <t>C200</t>
+    <t>C300, C304</t>
   </si>
   <si>
     <t>Capacitor</t>
   </si>
   <si>
+    <t>C 10nF 0402 16V</t>
+  </si>
+  <si>
+    <t>CAP CER 10000PF 16V Y5V 0402</t>
+  </si>
+  <si>
+    <t>Samsung Electro-Mechanics</t>
+  </si>
+  <si>
+    <t>CL05F103ZO5NNNC</t>
+  </si>
+  <si>
+    <t>CAP_10nF_16V_0402</t>
+  </si>
+  <si>
+    <t>Digi-Key</t>
+  </si>
+  <si>
+    <t>1276-1738-1-ND</t>
+  </si>
+  <si>
+    <t>C307, C308</t>
+  </si>
+  <si>
+    <t>C 5.6pF 0402 50V</t>
+  </si>
+  <si>
+    <t>CAP CER 5.6PF 50V C0G/NP0 0402</t>
+  </si>
+  <si>
+    <t>CL05C5R6DB5NNNC</t>
+  </si>
+  <si>
+    <t>CAP_5.6PF_50V_0402</t>
+  </si>
+  <si>
+    <t>1276-1712-1-ND</t>
+  </si>
+  <si>
+    <t>C200, C301, C302, C303</t>
+  </si>
+  <si>
     <t>C 1nF 0402 50V</t>
   </si>
   <si>
@@ -81,33 +123,9 @@
     <t>CAP_1nF_50V_0402</t>
   </si>
   <si>
-    <t>Digi-Key</t>
-  </si>
-  <si>
     <t>490-6190-1-ND</t>
   </si>
   <si>
-    <t>C307, C308</t>
-  </si>
-  <si>
-    <t>C 5.6pF 0402 50V</t>
-  </si>
-  <si>
-    <t>CAP CER 5.6PF 50V C0G/NP0 0402</t>
-  </si>
-  <si>
-    <t>Samsung Electro-Mechanics</t>
-  </si>
-  <si>
-    <t>CL05C5R6DB5NNNC</t>
-  </si>
-  <si>
-    <t>CAP_5.6PF_50V_0402</t>
-  </si>
-  <si>
-    <t>1276-1712-1-ND</t>
-  </si>
-  <si>
     <t>C201, C202, C203, C208</t>
   </si>
   <si>
@@ -129,24 +147,6 @@
     <t>587-5869-1-ND</t>
   </si>
   <si>
-    <t>C300, C301, C302, C303, C304</t>
-  </si>
-  <si>
-    <t>C 10nF 0402 16V</t>
-  </si>
-  <si>
-    <t>CAP CER 10000PF 16V Y5V 0402</t>
-  </si>
-  <si>
-    <t>CL05F103ZO5NNNC</t>
-  </si>
-  <si>
-    <t>CAP_10nF_16V_0402</t>
-  </si>
-  <si>
-    <t>1276-1738-1-ND</t>
-  </si>
-  <si>
     <t>C204, C205, C206, C207, C209, C305, C306, C400</t>
   </si>
   <si>
@@ -810,7 +810,25 @@
     <t>311-100KJRCT-ND</t>
   </si>
   <si>
-    <t>R203, R205, R208, R209, R210, R214, R215, R300, R301, R302, R303, R304, R305, R306, R307, R312, R319, R320</t>
+    <t>R200, R201, R216, R301, R302, R303, R304, R305, R307, R310, R315, R319, R321</t>
+  </si>
+  <si>
+    <t>R 270k 0402</t>
+  </si>
+  <si>
+    <t>RES 270K OHM 1% 1/16W 0402</t>
+  </si>
+  <si>
+    <t>RC0402FR-07270KL</t>
+  </si>
+  <si>
+    <t>R_270k_0402</t>
+  </si>
+  <si>
+    <t>311-270KLRCT-ND</t>
+  </si>
+  <si>
+    <t>R203, R205, R208, R209, R210, R214, R215, R300, R306, R312, R313, R314, R320</t>
   </si>
   <si>
     <t>R 10k 0402</t>
@@ -864,25 +882,7 @@
     <t>RMCF0402ZT0R00CT-ND</t>
   </si>
   <si>
-    <t>R200, R201, R216, R310</t>
-  </si>
-  <si>
-    <t>R 270k 0402</t>
-  </si>
-  <si>
-    <t>RES 270K OHM 1% 1/16W 0402</t>
-  </si>
-  <si>
-    <t>RC0402FR-07270KL</t>
-  </si>
-  <si>
-    <t>R_270k_0402</t>
-  </si>
-  <si>
-    <t>311-270KLRCT-ND</t>
-  </si>
-  <si>
-    <t>R204, R206, R207, R308, R309, R311, R313, R314</t>
+    <t>R204, R206, R207, R308, R309, R311</t>
   </si>
   <si>
     <t>R 2k 0402</t>
@@ -900,7 +900,7 @@
     <t>RMCF0402FT2K00CT-ND</t>
   </si>
   <si>
-    <t>R202, R315, R316, R317, R318, R321, R322, R323, R324</t>
+    <t>R202, R316, R317, R318, R322, R323, R324</t>
   </si>
   <si>
     <t>R 100R 0402</t>
@@ -1358,7 +1358,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0C4F5D5-517E-4EF1-A569-6450CD80B884}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9947B9A9-DB48-4A7C-9B3D-067309FD27C0}">
   <dimension ref="A1:J45"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -1409,7 +1409,7 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>10</v>
@@ -1456,19 +1456,19 @@
         <v>21</v>
       </c>
       <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="H3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="I3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -1476,51 +1476,51 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="3" t="s">
         <v>31</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="F5" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>22</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>36</v>
@@ -1552,7 +1552,7 @@
         <v>41</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="G6" s="3" t="s">
         <v>42</v>
@@ -2529,7 +2529,7 @@
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>260</v>
@@ -2561,7 +2561,7 @@
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
-        <v>2</v>
+        <v>13</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>266</v>
@@ -2576,7 +2576,7 @@
         <v>268</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>242</v>
+        <v>256</v>
       </c>
       <c r="G38" s="3" t="s">
         <v>269</v>
@@ -2593,7 +2593,7 @@
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>272</v>
@@ -2625,7 +2625,7 @@
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>278</v>
@@ -2640,7 +2640,7 @@
         <v>280</v>
       </c>
       <c r="F40" s="3" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="G40" s="3" t="s">
         <v>281</v>
@@ -2657,7 +2657,7 @@
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>284</v>
@@ -2689,7 +2689,7 @@
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>290</v>

</xml_diff>